<commit_message>
fixed MSA wrongly associated with COP
</commit_message>
<xml_diff>
--- a/data/raw/pmar1_survey_site_data.xlsx
+++ b/data/raw/pmar1_survey_site_data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="117">
   <si>
     <t>sample_site</t>
   </si>
@@ -314,6 +314,18 @@
     <t>The beach in front of the TAMUCC</t>
   </si>
   <si>
+    <t>CLP</t>
+  </si>
+  <si>
+    <t>Cole Park</t>
+  </si>
+  <si>
+    <t>27.776309, -97.391421</t>
+  </si>
+  <si>
+    <t>At edge of park near marina by seawall</t>
+  </si>
+  <si>
     <t>Site_Code</t>
   </si>
   <si>
@@ -330,15 +342,6 @@
   </si>
   <si>
     <t>La Salle Monument</t>
-  </si>
-  <si>
-    <t>CLP</t>
-  </si>
-  <si>
-    <t>27.776309, -97.391421</t>
-  </si>
-  <si>
-    <t>Cole Park</t>
   </si>
   <si>
     <t>North_Lyndon_Copano</t>
@@ -1058,6 +1061,29 @@
         <v>99</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1082,7 +1108,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -1125,7 +1151,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>31</v>
@@ -1137,7 +1163,7 @@
         <v>33</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4">
@@ -1185,7 +1211,7 @@
         <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>17</v>
@@ -1194,15 +1220,15 @@
         <v>18</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>97</v>
@@ -1214,10 +1240,10 @@
         <v>56</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8">
@@ -1225,7 +1251,7 @@
         <v>59</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>62</v>
@@ -1234,7 +1260,7 @@
         <v>63</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>65</v>
@@ -1245,7 +1271,7 @@
         <v>81</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>62</v>
@@ -1265,7 +1291,7 @@
         <v>45</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>48</v>
@@ -1285,7 +1311,7 @@
         <v>77</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>24</v>
@@ -1305,7 +1331,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>24</v>
@@ -1325,7 +1351,7 @@
         <v>86</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>31</v>

</xml_diff>